<commit_message>
emilia user story 3 return_inventory 19/12
</commit_message>
<xml_diff>
--- a/workOnExcel/Inventory.xlsx
+++ b/workOnExcel/Inventory.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21029"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emiliazorin\PycharmProjects\EMILIA\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35D8FF89-7BB0-45F0-9268-63D5EEEA5374}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="12" windowWidth="16092" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="inventory1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -37,7 +31,7 @@
     <t>color</t>
   </si>
   <si>
-    <t>shirts</t>
+    <t>jeans</t>
   </si>
   <si>
     <t>s/m/l</t>
@@ -46,9 +40,6 @@
     <t>black</t>
   </si>
   <si>
-    <t>jeans</t>
-  </si>
-  <si>
     <t>shoes</t>
   </si>
   <si>
@@ -58,27 +49,30 @@
     <t>shirt</t>
   </si>
   <si>
-    <t>s/m</t>
-  </si>
-  <si>
-    <t>red</t>
-  </si>
-  <si>
-    <t>we</t>
-  </si>
-  <si>
-    <t>dc</t>
+    <t>white</t>
+  </si>
+  <si>
+    <t>shorts</t>
+  </si>
+  <si>
+    <t>blue</t>
+  </si>
+  <si>
+    <t>hats</t>
+  </si>
+  <si>
+    <t>brown</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -111,19 +105,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="ערכת נושא Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -165,7 +151,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -197,27 +183,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -249,24 +217,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -442,16 +392,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -468,9 +416,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
@@ -485,9 +433,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
         <v>8</v>
@@ -502,9 +450,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
         <v>9</v>
@@ -519,9 +467,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
         <v>10</v>
@@ -530,41 +478,41 @@
         <v>6</v>
       </c>
       <c r="D5">
+        <v>6</v>
+      </c>
+      <c r="E5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6">
         <v>10</v>
-      </c>
-      <c r="E5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6">
-        <v>34</v>
       </c>
       <c r="E6" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="A7">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C7" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="D7">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E7" t="s">
         <v>15</v>

</xml_diff>

<commit_message>
emilia upadated the Inventory.xlsx
</commit_message>
<xml_diff>
--- a/workOnExcel/Inventory.xlsx
+++ b/workOnExcel/Inventory.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21029"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emiliazorin\Desktop\Yesodot!!!\Group2_Yesodot\workOnExcel\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03FBC956-E99E-4FA8-8ABD-8D9D05EC7221}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="12" windowWidth="16092" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="inventory1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="18">
   <si>
     <t>product code</t>
   </si>
@@ -58,21 +64,27 @@
     <t>blue</t>
   </si>
   <si>
-    <t>hats</t>
-  </si>
-  <si>
-    <t>brown</t>
+    <t>price</t>
+  </si>
+  <si>
+    <t>shirts</t>
+  </si>
+  <si>
+    <t>belts</t>
+  </si>
+  <si>
+    <t>red</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -105,11 +117,19 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="ערכת נושא Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -151,7 +171,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -183,9 +203,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -217,6 +255,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -392,14 +448,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:F8"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -415,30 +473,36 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="C2" t="s">
         <v>6</v>
       </c>
       <c r="D2">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="F2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C3" t="s">
         <v>6</v>
@@ -449,13 +513,16 @@
       <c r="E3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:5">
+      <c r="F3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s">
         <v>6</v>
@@ -466,56 +533,88 @@
       <c r="E4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:5">
+      <c r="F4">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5">
         <v>10</v>
       </c>
-      <c r="C5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5">
-        <v>6</v>
-      </c>
       <c r="E5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6">
+        <v>34</v>
+      </c>
+      <c r="E6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7">
+        <v>6</v>
+      </c>
+      <c r="E7" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6">
+      <c r="F7">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8">
         <v>7</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B8" t="s">
         <v>12</v>
       </c>
-      <c r="C6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6">
+      <c r="C8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8">
         <v>10</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E8" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7">
-        <v>8</v>
-      </c>
-      <c r="B7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7">
-        <v>10</v>
-      </c>
-      <c r="E7" t="s">
-        <v>15</v>
+      <c r="F8">
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
function sell_items+ delete items from sell
</commit_message>
<xml_diff>
--- a/workOnExcel/Inventory.xlsx
+++ b/workOnExcel/Inventory.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21029"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emiliazorin\PycharmProjects\EMILIA\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35D8FF89-7BB0-45F0-9268-63D5EEEA5374}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="12" windowWidth="16092" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="12" windowWidth="16092" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="inventory1" sheetId="1" r:id="rId1"/>
@@ -20,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="17">
   <si>
     <t>product code</t>
   </si>
@@ -68,12 +62,15 @@
   </si>
   <si>
     <t>dc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">price </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -165,7 +162,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -198,26 +195,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -250,23 +230,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -442,16 +405,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.296875" customWidth="1"/>
+    <col min="2" max="2" width="15.796875" customWidth="1"/>
+    <col min="3" max="3" width="12.5" customWidth="1"/>
+    <col min="4" max="4" width="11" customWidth="1"/>
+    <col min="5" max="5" width="17.5" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -467,8 +437,11 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -484,8 +457,11 @@
       <c r="E2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2">
+        <v>89.9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -501,8 +477,11 @@
       <c r="E3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -518,8 +497,11 @@
       <c r="E4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F4">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -535,8 +517,11 @@
       <c r="E5" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F5">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -552,8 +537,11 @@
       <c r="E6" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F6">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -568,6 +556,9 @@
       </c>
       <c r="E7" t="s">
         <v>15</v>
+      </c>
+      <c r="F7">
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
emilia i put in comment  a few print lines inside function
</commit_message>
<xml_diff>
--- a/workOnExcel/Inventory.xlsx
+++ b/workOnExcel/Inventory.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="15">
   <si>
     <t>product code</t>
   </si>
@@ -59,12 +59,6 @@
   </si>
   <si>
     <t>red</t>
-  </si>
-  <si>
-    <t>we</t>
-  </si>
-  <si>
-    <t>dc</t>
   </si>
 </sst>
 </file>
@@ -433,7 +427,7 @@
         <v>7</v>
       </c>
       <c r="D2">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="E2" t="s">
         <v>8</v>
@@ -473,7 +467,7 @@
         <v>7</v>
       </c>
       <c r="D4">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E4" t="s">
         <v>8</v>
@@ -493,7 +487,7 @@
         <v>7</v>
       </c>
       <c r="D5">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E5" t="s">
         <v>8</v>
@@ -530,13 +524,13 @@
         <v>12</v>
       </c>
       <c r="C7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D7">
         <v>6</v>
       </c>
       <c r="E7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F7">
         <v>50</v>

</xml_diff>

<commit_message>
story number: 10,21 - cancel sale, shir bar , 31.12.18
</commit_message>
<xml_diff>
--- a/workOnExcel/Inventory.xlsx
+++ b/workOnExcel/Inventory.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
   <si>
     <t>product code</t>
   </si>
@@ -22,43 +22,40 @@
     <t>name</t>
   </si>
   <si>
-    <t>size</t>
-  </si>
-  <si>
-    <t>amount</t>
+    <t>account</t>
   </si>
   <si>
     <t>color</t>
   </si>
   <si>
-    <t xml:space="preserve">price </t>
+    <t>price</t>
   </si>
   <si>
     <t>shirts</t>
   </si>
   <si>
-    <t>s/m/l</t>
-  </si>
-  <si>
     <t>black</t>
   </si>
   <si>
     <t>jeans</t>
   </si>
   <si>
+    <t>blue</t>
+  </si>
+  <si>
     <t>shoes</t>
   </si>
   <si>
     <t>coats</t>
   </si>
   <si>
-    <t>shirt</t>
-  </si>
-  <si>
-    <t>s/m</t>
+    <t xml:space="preserve">brown </t>
   </si>
   <si>
     <t>red</t>
+  </si>
+  <si>
+    <t>white</t>
   </si>
 </sst>
 </file>
@@ -390,13 +387,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -412,127 +409,106 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2">
+        <v>15</v>
+      </c>
+      <c r="D2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2">
-        <v>11</v>
-      </c>
-      <c r="E2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2">
+      <c r="E2">
         <v>89.90000000000001</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:5">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" t="s">
         <v>7</v>
       </c>
-      <c r="D3">
-        <v>10</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="C3">
+        <v>14</v>
+      </c>
+      <c r="D3" t="s">
         <v>8</v>
       </c>
-      <c r="F3">
+      <c r="E3">
         <v>200</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:5">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4">
+        <v>9</v>
+      </c>
+      <c r="C4">
         <v>8</v>
       </c>
-      <c r="E4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F4">
+      <c r="D4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4">
         <v>250</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:5">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5">
+        <v>9</v>
+      </c>
+      <c r="D5" t="s">
         <v>11</v>
       </c>
-      <c r="C5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5">
-        <v>9</v>
-      </c>
-      <c r="E5" t="s">
-        <v>8</v>
-      </c>
-      <c r="F5">
+      <c r="E5">
         <v>350</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:5">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>34</v>
+      </c>
+      <c r="D6" t="s">
         <v>12</v>
       </c>
-      <c r="C6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6">
-        <v>34</v>
-      </c>
-      <c r="E6" t="s">
-        <v>14</v>
-      </c>
-      <c r="F6">
+      <c r="E6">
         <v>70</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:5">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7">
+        <v>6</v>
+      </c>
+      <c r="D7" t="s">
         <v>13</v>
       </c>
-      <c r="D7">
-        <v>6</v>
-      </c>
-      <c r="E7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F7">
+      <c r="E7">
         <v>50</v>
       </c>
     </row>

</xml_diff>